<commit_message>
Corrected error for columnwise timeseries with one label row. Updated the testset.
</commit_message>
<xml_diff>
--- a/pkg/tests/testthat/read_ts/xlsx/example5.xlsx
+++ b/pkg/tests/testthat/read_ts/xlsx/example5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="first_sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -189,7 +189,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.4183673469388"/>
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="114.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -221,14 +221,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.42857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.29591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,12 +317,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
read_ts_xls has an argument warn_num_text. The default is TRUE.
</commit_message>
<xml_diff>
--- a/pkg/tests/testthat/read_ts/xlsx/example5.xlsx
+++ b/pkg/tests/testthat/read_ts/xlsx/example5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="first_sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">The data is on the next sheet </t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">Timeseries b in euros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxx</t>
   </si>
   <si>
     <t xml:space="preserve">xxxx</t>
@@ -189,7 +192,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="114.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -215,20 +218,20 @@
   </sheetPr>
   <dimension ref="A3:J8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.29591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -274,19 +277,22 @@
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E7" s="0" t="s">
+        <v>10</v>
+      </c>
       <c r="J7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>10</v>
@@ -316,14 +322,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="218" zoomScaleNormal="218" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>